<commit_message>
fully implement current usb-side message protocol
still missing code to receive commands from the cloud, but at this point
that should be pretty easy to add.
</commit_message>
<xml_diff>
--- a/message scheme.xlsx
+++ b/message scheme.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="112">
   <si>
     <t>byte #</t>
   </si>
@@ -81,12 +81,6 @@
     <t>int32</t>
   </si>
   <si>
-    <t>float32</t>
-  </si>
-  <si>
-    <t>float64</t>
-  </si>
-  <si>
     <t>type number</t>
   </si>
   <si>
@@ -105,9 +99,6 @@
     <t>0-3</t>
   </si>
   <si>
-    <t>0-7</t>
-  </si>
-  <si>
     <t>JSON</t>
   </si>
   <si>
@@ -129,12 +120,6 @@
     <t>etc</t>
   </si>
   <si>
-    <t>byte stream</t>
-  </si>
-  <si>
-    <t>number of bytes</t>
-  </si>
-  <si>
     <t>L+1…M</t>
   </si>
   <si>
@@ -144,9 +129,6 @@
     <t>M+L+1…2*M+L</t>
   </si>
   <si>
-    <t>raw bytes</t>
-  </si>
-  <si>
     <t>generic data</t>
   </si>
   <si>
@@ -283,6 +265,93 @@
   </si>
   <si>
     <t>boolean</t>
+  </si>
+  <si>
+    <t>message IDs</t>
+  </si>
+  <si>
+    <t>0x00</t>
+  </si>
+  <si>
+    <t>announce unique device name (string)</t>
+  </si>
+  <si>
+    <t>subscribe</t>
+  </si>
+  <si>
+    <t>unsubscribe</t>
+  </si>
+  <si>
+    <t>0x10</t>
+  </si>
+  <si>
+    <t>refrigerator.filterAlert</t>
+  </si>
+  <si>
+    <t>0x12</t>
+  </si>
+  <si>
+    <t>0x13</t>
+  </si>
+  <si>
+    <t>0x14</t>
+  </si>
+  <si>
+    <t>0x15</t>
+  </si>
+  <si>
+    <t>0x16</t>
+  </si>
+  <si>
+    <t>0x17</t>
+  </si>
+  <si>
+    <t>0x18</t>
+  </si>
+  <si>
+    <t>0x19</t>
+  </si>
+  <si>
+    <t>0x1A</t>
+  </si>
+  <si>
+    <t>refrigerator.filterExpirationStatus</t>
+  </si>
+  <si>
+    <t>refrigerator.commandFeatures</t>
+  </si>
+  <si>
+    <t>refrigerator.temperatureAlert</t>
+  </si>
+  <si>
+    <t>refrigerator.displayTemperature</t>
+  </si>
+  <si>
+    <t>refrigerator.setpointTemperature</t>
+  </si>
+  <si>
+    <t>refrigerator.doorAlarmAlert</t>
+  </si>
+  <si>
+    <t>refrigerator.iceMakerBucketStatus</t>
+  </si>
+  <si>
+    <t>refrigerator.odorFilterExpirationStatus</t>
+  </si>
+  <si>
+    <t>refrigerator.doorState</t>
+  </si>
+  <si>
+    <t>refrigerator.doorBoard.information</t>
+  </si>
+  <si>
+    <t>reserve 0x00-0x3F</t>
+  </si>
+  <si>
+    <t>0x06</t>
+  </si>
+  <si>
+    <t>length 6</t>
   </si>
 </sst>
 </file>
@@ -365,22 +434,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -683,10 +755,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AC41"/>
+  <dimension ref="A1:AA45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -694,41 +766,41 @@
     <col min="3" max="3" width="19.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="J7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0</v>
       </c>
@@ -736,10 +808,10 @@
         <v>2</v>
       </c>
       <c r="J8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -747,37 +819,37 @@
         <v>12</v>
       </c>
       <c r="J9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="K10" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="L10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="K11" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="L11">
         <v>314</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -791,78 +863,72 @@
         <v>5</v>
       </c>
       <c r="J13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C14" s="1">
         <v>1</v>
       </c>
       <c r="D14" t="s">
+        <v>66</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="L14" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="J14" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="M14" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="N14" s="4" t="s">
+      <c r="M14" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N14" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q14" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="R14" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="S14" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="T14" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="U14" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="V14" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="O14" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="P14" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q14" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="R14" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="S14" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="T14" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="U14" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="V14" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="W14" s="4" t="s">
-        <v>87</v>
+      <c r="W14" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="X14" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y14" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="Z14" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA14" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="AB14" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC14" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="Y14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z14" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA14" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C15" s="1" t="s">
         <v>7</v>
       </c>
@@ -870,116 +936,108 @@
         <v>6</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K15" s="3"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="K15" s="6"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
       <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="4"/>
-      <c r="S15" s="4"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
       <c r="T15" s="4"/>
-      <c r="U15" s="4"/>
-      <c r="V15" s="3"/>
-      <c r="W15" s="4"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="7"/>
+      <c r="W15" s="7"/>
       <c r="X15" s="4"/>
-      <c r="Y15" s="4"/>
-      <c r="Z15" s="4"/>
-      <c r="AA15" s="3"/>
-      <c r="AB15" s="4"/>
-      <c r="AC15" s="6"/>
-    </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="Y15" s="3"/>
+      <c r="Z15" s="6"/>
+      <c r="AA15" s="9"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
         <v>10</v>
       </c>
-      <c r="K16" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
       <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
-      <c r="Q16" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="R16" s="4"/>
-      <c r="S16" s="4"/>
+      <c r="P16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
       <c r="T16" s="4"/>
-      <c r="U16" s="4"/>
-      <c r="V16" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="W16" s="4"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="7"/>
+      <c r="W16" s="7"/>
       <c r="X16" s="4"/>
-      <c r="Y16" s="4"/>
-      <c r="Z16" s="4"/>
-      <c r="AA16" s="3" t="s">
+      <c r="Y16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="AB16" s="4"/>
-      <c r="AC16" s="4"/>
-    </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="Z16" s="6"/>
+      <c r="AA16" s="4"/>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C17" s="1"/>
       <c r="D17" t="s">
         <v>11</v>
       </c>
-      <c r="L17" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="M17" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="N17" s="4" t="s">
-        <v>83</v>
+      <c r="K17" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="M17" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="N17" s="7" t="s">
+        <v>57</v>
       </c>
       <c r="O17" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="P17" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="R17" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q17" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="R17" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="S17" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="T17" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="S17" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="T17" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="U17" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="W17" s="4" t="s">
-        <v>81</v>
+      <c r="U17" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="V17" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="W17" s="7" t="s">
+        <v>77</v>
       </c>
       <c r="X17" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="Y17" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="Z17" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="AB17" s="7">
+        <v>58</v>
+      </c>
+      <c r="Z17" s="11">
         <v>314</v>
       </c>
-      <c r="AC17" s="7"/>
-    </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AA17" s="10"/>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -993,48 +1051,51 @@
         <v>14</v>
       </c>
       <c r="J19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C20" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J20" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C21" s="1"/>
       <c r="J21" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="L21" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="M21" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="N21" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="O21" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="P21" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q21" s="10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="N21" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="O21" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="P21" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q21" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="R21" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -1045,20 +1106,21 @@
         <v>0</v>
       </c>
       <c r="D22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="K22" s="3"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="10"/>
-    </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="L22" s="3"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="6"/>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -1069,19 +1131,22 @@
         <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="L23" s="8"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="10"/>
-    </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M23" s="4"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="6"/>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -1089,31 +1154,31 @@
         <v>5</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D24" t="s">
-        <v>26</v>
-      </c>
-      <c r="L24" s="8">
+        <v>24</v>
+      </c>
+      <c r="M24" s="4">
         <v>2</v>
       </c>
-      <c r="M24" s="9">
+      <c r="N24" s="5">
         <v>-5</v>
       </c>
-      <c r="N24" s="9">
+      <c r="O24" s="5">
         <v>31</v>
       </c>
-      <c r="O24" s="9">
+      <c r="P24" s="5">
         <v>45</v>
       </c>
-      <c r="P24" s="9">
+      <c r="Q24" s="5">
         <v>-120</v>
       </c>
-      <c r="Q24" s="10">
+      <c r="R24" s="6">
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -1121,13 +1186,13 @@
         <v>6</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D25" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -1135,13 +1200,13 @@
         <v>7</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -1149,137 +1214,196 @@
         <v>8</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="C28" s="1"/>
+      <c r="J28" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>9</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0</v>
+      </c>
+      <c r="D29" t="s">
         <v>28</v>
       </c>
-      <c r="D27" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28">
-        <v>9</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D28" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>22</v>
-      </c>
-      <c r="B29">
+      <c r="J29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="C30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="C31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" t="s">
+        <v>30</v>
+      </c>
+      <c r="J31" t="s">
+        <v>84</v>
+      </c>
+      <c r="K31" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="C32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" t="s">
+        <v>31</v>
+      </c>
+      <c r="J32" t="s">
+        <v>47</v>
+      </c>
+      <c r="K32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C33" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" t="s">
+        <v>32</v>
+      </c>
+      <c r="J33" t="s">
+        <v>46</v>
+      </c>
+      <c r="K33" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C34" s="1"/>
+      <c r="D34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C35" s="1"/>
+      <c r="J35" t="s">
+        <v>88</v>
+      </c>
+      <c r="K35" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36">
         <v>10</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D29" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="C30" s="1"/>
-    </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31">
-        <v>11</v>
-      </c>
-      <c r="C31" s="1">
+      <c r="C36">
         <v>0</v>
       </c>
-      <c r="D31" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="C32" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C33" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C34" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D34" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C35" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D35" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C36" s="1"/>
       <c r="D36" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="J36" t="s">
+        <v>45</v>
+      </c>
+      <c r="K36" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C37" s="1"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38">
-        <v>12</v>
-      </c>
-      <c r="C38" s="1">
-        <v>0</v>
-      </c>
-      <c r="D38" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C39" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D39" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>88</v>
-      </c>
-      <c r="B41">
-        <v>13</v>
-      </c>
-      <c r="C41">
-        <v>0</v>
-      </c>
-      <c r="D41" t="s">
-        <v>26</v>
+      <c r="J37" t="s">
+        <v>90</v>
+      </c>
+      <c r="K37" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J38" t="s">
+        <v>91</v>
+      </c>
+      <c r="K38" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J39" t="s">
+        <v>92</v>
+      </c>
+      <c r="K39" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J40" t="s">
+        <v>93</v>
+      </c>
+      <c r="K40" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J41" t="s">
+        <v>94</v>
+      </c>
+      <c r="K41" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J42" t="s">
+        <v>95</v>
+      </c>
+      <c r="K42" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J43" t="s">
+        <v>96</v>
+      </c>
+      <c r="K43" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J44" t="s">
+        <v>97</v>
+      </c>
+      <c r="K44" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J45" t="s">
+        <v>98</v>
+      </c>
+      <c r="K45" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="AB17:AC17"/>
+    <mergeCell ref="Z17:AA17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finish data translator, fix random bugs
</commit_message>
<xml_diff>
--- a/message scheme.xlsx
+++ b/message scheme.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="163">
   <si>
     <t>byte #</t>
   </si>
@@ -285,9 +285,6 @@
     <t>0x10</t>
   </si>
   <si>
-    <t>refrigerator.filterAlert</t>
-  </si>
-  <si>
     <t>0x12</t>
   </si>
   <si>
@@ -315,56 +312,218 @@
     <t>0x1A</t>
   </si>
   <si>
-    <t>refrigerator.filterExpirationStatus</t>
-  </si>
-  <si>
-    <t>refrigerator.commandFeatures</t>
-  </si>
-  <si>
-    <t>refrigerator.temperatureAlert</t>
-  </si>
-  <si>
-    <t>refrigerator.displayTemperature</t>
-  </si>
-  <si>
-    <t>refrigerator.setpointTemperature</t>
-  </si>
-  <si>
-    <t>refrigerator.doorAlarmAlert</t>
-  </si>
-  <si>
-    <t>refrigerator.iceMakerBucketStatus</t>
-  </si>
-  <si>
-    <t>refrigerator.odorFilterExpirationStatus</t>
-  </si>
-  <si>
-    <t>refrigerator.doorState</t>
-  </si>
-  <si>
-    <t>refrigerator.doorBoard.information</t>
-  </si>
-  <si>
-    <t>reserve 0x00-0x3F</t>
-  </si>
-  <si>
     <t>0x06</t>
   </si>
   <si>
     <t>length 6</t>
+  </si>
+  <si>
+    <t>messages to the cloud have the fields</t>
+  </si>
+  <si>
+    <t>devId</t>
+  </si>
+  <si>
+    <t>device</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>device index on the fridge</t>
+  </si>
+  <si>
+    <t>manufacturere provided "name" of the device, e.g. "MilkMinder"</t>
+  </si>
+  <si>
+    <t>message type</t>
+  </si>
+  <si>
+    <t>whatever data</t>
+  </si>
+  <si>
+    <t>waterFilterCalendarTimer</t>
+  </si>
+  <si>
+    <t>waterFilterHoursRemaining</t>
+  </si>
+  <si>
+    <t>filterAlert</t>
+  </si>
+  <si>
+    <t>waterUsageTimer</t>
+  </si>
+  <si>
+    <t>waterFilterUsageTimePercentUsed</t>
+  </si>
+  <si>
+    <t>waterFilterOunces Remaining</t>
+  </si>
+  <si>
+    <t>commandFeatures</t>
+  </si>
+  <si>
+    <t>temperatureAlert</t>
+  </si>
+  <si>
+    <t>freshFoodDisplayTemperature</t>
+  </si>
+  <si>
+    <t>freezerDisplayTemperature</t>
+  </si>
+  <si>
+    <t>freshFoodSetpointTemperature</t>
+  </si>
+  <si>
+    <t>freezerSetpointTemperature</t>
+  </si>
+  <si>
+    <t>doorAlarmAlert</t>
+  </si>
+  <si>
+    <t>iceMakerBucketStatus</t>
+  </si>
+  <si>
+    <t>odorFilterCalendarTimer</t>
+  </si>
+  <si>
+    <t>odorFilterPercentUsed</t>
+  </si>
+  <si>
+    <t>odorFilterHoursRemaining</t>
+  </si>
+  <si>
+    <t>doorState</t>
+  </si>
+  <si>
+    <t>dcSwitchState</t>
+  </si>
+  <si>
+    <t>acInputState</t>
+  </si>
+  <si>
+    <t>0x20</t>
+  </si>
+  <si>
+    <t>0x21</t>
+  </si>
+  <si>
+    <t>0x22</t>
+  </si>
+  <si>
+    <t>0x23</t>
+  </si>
+  <si>
+    <t>0x24</t>
+  </si>
+  <si>
+    <t>0x25</t>
+  </si>
+  <si>
+    <t>0x26</t>
+  </si>
+  <si>
+    <t>0x27</t>
+  </si>
+  <si>
+    <t>0x28</t>
+  </si>
+  <si>
+    <t>0x29</t>
+  </si>
+  <si>
+    <t>reserve 0x00-0x4F</t>
+  </si>
+  <si>
+    <t>0x1B</t>
+  </si>
+  <si>
+    <t>0x1C</t>
+  </si>
+  <si>
+    <t>0x1D</t>
+  </si>
+  <si>
+    <t>0x1E</t>
+  </si>
+  <si>
+    <t>0x1F</t>
+  </si>
+  <si>
+    <t>0x2A</t>
+  </si>
+  <si>
+    <t>0x2B</t>
+  </si>
+  <si>
+    <t>0x2C</t>
+  </si>
+  <si>
+    <t>U8</t>
+  </si>
+  <si>
+    <t>U16</t>
+  </si>
+  <si>
+    <t>waterFilterCalendarPercentUsed</t>
+  </si>
+  <si>
+    <t>U32</t>
+  </si>
+  <si>
+    <t>iceMakerMoldThermistorTemperature</t>
+  </si>
+  <si>
+    <t>iceCabinetThermistorTemperature</t>
+  </si>
+  <si>
+    <t>hotWaterThermistor1Temperature</t>
+  </si>
+  <si>
+    <t>hotWaterThermistor2Temperature</t>
+  </si>
+  <si>
+    <t>dctSwitchState</t>
+  </si>
+  <si>
+    <t>relayStatus</t>
+  </si>
+  <si>
+    <t>ductDoorStatus</t>
+  </si>
+  <si>
+    <t>iceMakerStateSelection</t>
+  </si>
+  <si>
+    <t>0x2D</t>
+  </si>
+  <si>
+    <t>iceMakerOperationalState</t>
+  </si>
+  <si>
+    <t>message length in bytes (not including the 'length' byte itself)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -434,7 +593,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -447,10 +606,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -755,15 +915,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AA45"/>
+  <dimension ref="A1:AA64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.3">
@@ -772,57 +933,65 @@
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>25</v>
+      <c r="A2">
+        <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>71</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>37</v>
-      </c>
       <c r="J7" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>0</v>
-      </c>
-      <c r="B8" t="s">
-        <v>2</v>
+      <c r="A8" t="s">
+        <v>37</v>
       </c>
       <c r="J8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>3</v>
+      <c r="A9">
+        <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="J9" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
       <c r="K10" t="s">
         <v>41</v>
       </c>
@@ -839,39 +1008,33 @@
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" t="s">
-        <v>22</v>
-      </c>
       <c r="J12" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1">
-        <v>0</v>
-      </c>
-      <c r="D13" t="s">
-        <v>5</v>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
       </c>
       <c r="J13" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
       <c r="C14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>66</v>
+        <v>5</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>45</v>
@@ -929,11 +1092,11 @@
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="C15" s="1" t="s">
-        <v>7</v>
+      <c r="C15" s="1">
+        <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>27</v>
@@ -958,10 +1121,10 @@
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C16" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="K16" s="6"/>
       <c r="L16" s="7"/>
@@ -986,9 +1149,11 @@
       <c r="AA16" s="4"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="C17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="D17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K17" s="6" t="s">
         <v>75</v>
@@ -1032,46 +1197,49 @@
       <c r="Z17" s="11">
         <v>314</v>
       </c>
-      <c r="AA17" s="10"/>
+      <c r="AA17" s="12"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C18" s="1"/>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="C19" s="1">
-        <v>0</v>
-      </c>
-      <c r="D19" t="s">
-        <v>14</v>
-      </c>
+      <c r="C19" s="1"/>
       <c r="J19" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="C20" s="1" t="s">
-        <v>3</v>
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="J20" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="C21" s="1"/>
+      <c r="C21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" t="s">
+        <v>23</v>
+      </c>
       <c r="J21" s="2" t="s">
         <v>47</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="L21" s="3" t="s">
         <v>61</v>
@@ -1096,18 +1264,7 @@
       </c>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22">
-        <v>3</v>
-      </c>
-      <c r="C22" s="1">
-        <v>0</v>
-      </c>
-      <c r="D22" t="s">
-        <v>24</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="J22" s="2" t="s">
         <v>67</v>
       </c>
@@ -1122,10 +1279,10 @@
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C23" s="1">
         <v>0</v>
@@ -1134,7 +1291,7 @@
         <v>24</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="L23" s="3" t="s">
         <v>68</v>
@@ -1148,13 +1305,13 @@
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B24">
-        <v>5</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>25</v>
+        <v>4</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0</v>
       </c>
       <c r="D24" t="s">
         <v>24</v>
@@ -1180,10 +1337,10 @@
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B25">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>25</v>
@@ -1194,13 +1351,13 @@
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B26">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D26" t="s">
         <v>24</v>
@@ -1208,10 +1365,10 @@
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B27">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>26</v>
@@ -1221,42 +1378,60 @@
       </c>
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="C28" s="1"/>
+      <c r="A28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28">
+        <v>8</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" t="s">
+        <v>24</v>
+      </c>
       <c r="J28" t="s">
         <v>83</v>
       </c>
+      <c r="P28" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="C29" s="1"/>
+      <c r="J29" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>27</v>
       </c>
-      <c r="B29">
+      <c r="B30">
         <v>9</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C30" s="1">
         <v>0</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D30" t="s">
         <v>28</v>
       </c>
-      <c r="J29" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="C30" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" t="s">
-        <v>29</v>
+      <c r="P30" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C31" s="1" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="D31" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
       </c>
       <c r="J31" t="s">
         <v>84</v>
@@ -1264,13 +1439,22 @@
       <c r="K31" t="s">
         <v>85</v>
       </c>
+      <c r="P31" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C32" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D32" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
       </c>
       <c r="J32" t="s">
         <v>47</v>
@@ -1278,13 +1462,22 @@
       <c r="K32" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="P32" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C33" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D33" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="I33">
+        <v>2</v>
       </c>
       <c r="J33" t="s">
         <v>46</v>
@@ -1292,113 +1485,457 @@
       <c r="K33" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C34" s="1"/>
+      <c r="P33" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C34" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="D34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C35" s="1"/>
+      <c r="D35" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C35" s="1"/>
+      <c r="I35">
+        <v>16</v>
+      </c>
       <c r="J35" t="s">
         <v>88</v>
       </c>
       <c r="K35" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>82</v>
-      </c>
-      <c r="B36">
-        <v>10</v>
-      </c>
-      <c r="C36">
-        <v>0</v>
-      </c>
-      <c r="D36" t="s">
-        <v>24</v>
+        <v>111</v>
+      </c>
+      <c r="L35" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C36" s="1"/>
+      <c r="I36">
+        <v>17</v>
       </c>
       <c r="J36" t="s">
         <v>45</v>
       </c>
       <c r="K36" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C37" s="1"/>
+        <v>109</v>
+      </c>
+      <c r="L36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37">
+        <v>10</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37" t="s">
+        <v>24</v>
+      </c>
+      <c r="I37">
+        <v>18</v>
+      </c>
       <c r="J37" t="s">
+        <v>89</v>
+      </c>
+      <c r="K37" t="s">
+        <v>150</v>
+      </c>
+      <c r="L37" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C38" s="1"/>
+      <c r="I38">
+        <v>19</v>
+      </c>
+      <c r="J38" t="s">
         <v>90</v>
       </c>
-      <c r="K37" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="J38" t="s">
+      <c r="K38" t="s">
+        <v>110</v>
+      </c>
+      <c r="L38" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="I39">
+        <v>20</v>
+      </c>
+      <c r="J39" t="s">
         <v>91</v>
       </c>
-      <c r="K38" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="J39" t="s">
+      <c r="K39" t="s">
+        <v>112</v>
+      </c>
+      <c r="L39" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="I40">
+        <v>21</v>
+      </c>
+      <c r="J40" t="s">
         <v>92</v>
       </c>
-      <c r="K39" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="J40" t="s">
+      <c r="K40" t="s">
+        <v>113</v>
+      </c>
+      <c r="L40" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="I41">
+        <v>22</v>
+      </c>
+      <c r="J41" t="s">
         <v>93</v>
       </c>
-      <c r="K40" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="J41" t="s">
+      <c r="K41" t="s">
+        <v>114</v>
+      </c>
+      <c r="L41" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="I42">
+        <v>23</v>
+      </c>
+      <c r="J42" t="s">
         <v>94</v>
       </c>
-      <c r="K41" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="J42" t="s">
+      <c r="K42" t="s">
+        <v>115</v>
+      </c>
+      <c r="L42" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="I43">
+        <v>24</v>
+      </c>
+      <c r="J43" t="s">
         <v>95</v>
       </c>
-      <c r="K42" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="J43" t="s">
+      <c r="K43" t="s">
+        <v>116</v>
+      </c>
+      <c r="L43" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="I44">
+        <v>25</v>
+      </c>
+      <c r="J44" t="s">
         <v>96</v>
       </c>
-      <c r="K43" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="J44" t="s">
+      <c r="K44" t="s">
+        <v>117</v>
+      </c>
+      <c r="L44" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="I45">
+        <v>26</v>
+      </c>
+      <c r="J45" t="s">
         <v>97</v>
       </c>
-      <c r="K44" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="J45" t="s">
-        <v>98</v>
-      </c>
       <c r="K45" t="s">
-        <v>108</v>
+        <v>118</v>
+      </c>
+      <c r="L45" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="I46">
+        <v>27</v>
+      </c>
+      <c r="J46" t="s">
+        <v>140</v>
+      </c>
+      <c r="K46" t="s">
+        <v>119</v>
+      </c>
+      <c r="L46" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="I47">
+        <v>28</v>
+      </c>
+      <c r="J47" t="s">
+        <v>141</v>
+      </c>
+      <c r="K47" t="s">
+        <v>120</v>
+      </c>
+      <c r="L47" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="I48">
+        <v>29</v>
+      </c>
+      <c r="J48" t="s">
+        <v>142</v>
+      </c>
+      <c r="K48" t="s">
+        <v>121</v>
+      </c>
+      <c r="L48" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="49" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I49">
+        <v>30</v>
+      </c>
+      <c r="J49" t="s">
+        <v>143</v>
+      </c>
+      <c r="K49" t="s">
+        <v>122</v>
+      </c>
+      <c r="L49" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="50" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I50">
+        <v>31</v>
+      </c>
+      <c r="J50" t="s">
+        <v>144</v>
+      </c>
+      <c r="K50" t="s">
+        <v>123</v>
+      </c>
+      <c r="L50" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="51" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I51">
+        <v>32</v>
+      </c>
+      <c r="J51" t="s">
+        <v>129</v>
+      </c>
+      <c r="K51" t="s">
+        <v>124</v>
+      </c>
+      <c r="L51" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="52" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I52">
+        <v>33</v>
+      </c>
+      <c r="J52" t="s">
+        <v>130</v>
+      </c>
+      <c r="K52" t="s">
+        <v>125</v>
+      </c>
+      <c r="L52" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="53" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I53">
+        <v>34</v>
+      </c>
+      <c r="J53" t="s">
+        <v>131</v>
+      </c>
+      <c r="K53" t="s">
+        <v>126</v>
+      </c>
+      <c r="L53" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="54" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I54">
+        <v>35</v>
+      </c>
+      <c r="J54" t="s">
+        <v>132</v>
+      </c>
+      <c r="K54" t="s">
+        <v>127</v>
+      </c>
+      <c r="L54" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="55" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I55">
+        <v>36</v>
+      </c>
+      <c r="J55" t="s">
+        <v>133</v>
+      </c>
+      <c r="K55" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="L55" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="56" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I56">
+        <v>37</v>
+      </c>
+      <c r="J56" t="s">
+        <v>134</v>
+      </c>
+      <c r="K56" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="L56" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="57" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I57">
+        <v>38</v>
+      </c>
+      <c r="J57" t="s">
+        <v>135</v>
+      </c>
+      <c r="K57" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="L57" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="58" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I58">
+        <v>39</v>
+      </c>
+      <c r="J58" t="s">
+        <v>136</v>
+      </c>
+      <c r="K58" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="L58" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="59" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I59">
+        <v>40</v>
+      </c>
+      <c r="J59" t="s">
+        <v>137</v>
+      </c>
+      <c r="K59" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="L59" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="60" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I60">
+        <v>41</v>
+      </c>
+      <c r="J60" t="s">
+        <v>138</v>
+      </c>
+      <c r="K60" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="L60" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="61" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I61">
+        <v>42</v>
+      </c>
+      <c r="J61" t="s">
+        <v>145</v>
+      </c>
+      <c r="K61" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="L61" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="62" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I62">
+        <v>43</v>
+      </c>
+      <c r="J62" t="s">
+        <v>146</v>
+      </c>
+      <c r="K62" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="L62" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="63" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I63">
+        <v>44</v>
+      </c>
+      <c r="J63" t="s">
+        <v>147</v>
+      </c>
+      <c r="K63" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="L63" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="64" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I64">
+        <v>45</v>
+      </c>
+      <c r="J64" t="s">
+        <v>160</v>
+      </c>
+      <c r="K64" t="s">
+        <v>161</v>
+      </c>
+      <c r="L64" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add reference implementation on arduino
</commit_message>
<xml_diff>
--- a/message scheme.xlsx
+++ b/message scheme.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="165">
   <si>
     <t>byte #</t>
   </si>
@@ -505,6 +505,12 @@
   </si>
   <si>
     <t>message length in bytes (not including the 'length' byte itself)</t>
+  </si>
+  <si>
+    <t>define USB frame size</t>
+  </si>
+  <si>
+    <t>definitely send this one before subscribing to anything</t>
   </si>
 </sst>
 </file>
@@ -915,10 +921,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AA64"/>
+  <dimension ref="A1:AA65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="F9" workbookViewId="0">
+      <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -955,6 +961,7 @@
       <c r="B4" t="s">
         <v>1</v>
       </c>
+      <c r="G4" s="1"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -1499,38 +1506,41 @@
       <c r="D34" t="s">
         <v>32</v>
       </c>
+      <c r="I34">
+        <v>3</v>
+      </c>
+      <c r="J34" t="s">
+        <v>81</v>
+      </c>
+      <c r="K34" t="s">
+        <v>163</v>
+      </c>
+      <c r="L34" t="s">
+        <v>148</v>
+      </c>
+      <c r="M34" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C35" s="1"/>
       <c r="D35" t="s">
         <v>33</v>
       </c>
-      <c r="I35">
-        <v>16</v>
-      </c>
-      <c r="J35" t="s">
-        <v>88</v>
-      </c>
-      <c r="K35" t="s">
-        <v>111</v>
-      </c>
-      <c r="L35" t="s">
-        <v>148</v>
-      </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C36" s="1"/>
       <c r="I36">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J36" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="K36" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="L36" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.3">
@@ -1547,98 +1557,98 @@
         <v>24</v>
       </c>
       <c r="I37">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J37" t="s">
-        <v>89</v>
+        <v>45</v>
       </c>
       <c r="K37" t="s">
-        <v>150</v>
+        <v>109</v>
       </c>
       <c r="L37" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C38" s="1"/>
       <c r="I38">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J38" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K38" t="s">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="L38" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I39">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J39" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K39" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="L39" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I40">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J40" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K40" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L40" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I41">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J41" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K41" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L41" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I42">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K42" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L42" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I43">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J43" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K43" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L43" t="s">
         <v>148</v>
@@ -1646,13 +1656,13 @@
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I44">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K44" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L44" t="s">
         <v>148</v>
@@ -1660,13 +1670,13 @@
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I45">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J45" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K45" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L45" t="s">
         <v>148</v>
@@ -1674,13 +1684,13 @@
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I46">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J46" t="s">
-        <v>140</v>
+        <v>97</v>
       </c>
       <c r="K46" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L46" t="s">
         <v>148</v>
@@ -1688,13 +1698,13 @@
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I47">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J47" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K47" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L47" t="s">
         <v>148</v>
@@ -1702,13 +1712,13 @@
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I48">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J48" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K48" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L48" t="s">
         <v>148</v>
@@ -1716,13 +1726,13 @@
     </row>
     <row r="49" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I49">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J49" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K49" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L49" t="s">
         <v>148</v>
@@ -1730,41 +1740,41 @@
     </row>
     <row r="50" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I50">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J50" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K50" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L50" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="51" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I51">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J51" t="s">
-        <v>129</v>
+        <v>144</v>
       </c>
       <c r="K51" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L51" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="52" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I52">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J52" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K52" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L52" t="s">
         <v>148</v>
@@ -1772,13 +1782,13 @@
     </row>
     <row r="53" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I53">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J53" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K53" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L53" t="s">
         <v>148</v>
@@ -1786,13 +1796,13 @@
     </row>
     <row r="54" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I54">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J54" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K54" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L54" t="s">
         <v>148</v>
@@ -1800,13 +1810,13 @@
     </row>
     <row r="55" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I55">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J55" t="s">
-        <v>133</v>
-      </c>
-      <c r="K55" s="10" t="s">
-        <v>128</v>
+        <v>132</v>
+      </c>
+      <c r="K55" t="s">
+        <v>127</v>
       </c>
       <c r="L55" t="s">
         <v>148</v>
@@ -1814,27 +1824,27 @@
     </row>
     <row r="56" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I56">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J56" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K56" s="10" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="L56" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="57" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I57">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J57" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K57" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L57" t="s">
         <v>149</v>
@@ -1842,13 +1852,13 @@
     </row>
     <row r="58" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I58">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J58" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K58" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L58" t="s">
         <v>149</v>
@@ -1856,13 +1866,13 @@
     </row>
     <row r="59" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I59">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J59" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K59" s="10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L59" t="s">
         <v>149</v>
@@ -1870,27 +1880,27 @@
     </row>
     <row r="60" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I60">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J60" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K60" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L60" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="61" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I61">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J61" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="K61" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L61" t="s">
         <v>148</v>
@@ -1898,13 +1908,13 @@
     </row>
     <row r="62" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I62">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J62" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K62" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L62" t="s">
         <v>148</v>
@@ -1912,13 +1922,13 @@
     </row>
     <row r="63" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I63">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J63" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K63" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L63" t="s">
         <v>148</v>
@@ -1926,15 +1936,29 @@
     </row>
     <row r="64" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I64">
+        <v>44</v>
+      </c>
+      <c r="J64" t="s">
+        <v>147</v>
+      </c>
+      <c r="K64" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="L64" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="65" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I65">
         <v>45</v>
       </c>
-      <c r="J64" t="s">
+      <c r="J65" t="s">
         <v>160</v>
       </c>
-      <c r="K64" t="s">
+      <c r="K65" t="s">
         <v>161</v>
       </c>
-      <c r="L64" t="s">
+      <c r="L65" t="s">
         <v>148</v>
       </c>
     </row>

</xml_diff>

<commit_message>
switch from hid to cdc-acm
</commit_message>
<xml_diff>
--- a/message scheme.xlsx
+++ b/message scheme.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="163">
   <si>
     <t>byte #</t>
   </si>
@@ -505,12 +505,6 @@
   </si>
   <si>
     <t>message length in bytes (not including the 'length' byte itself)</t>
-  </si>
-  <si>
-    <t>define USB frame size</t>
-  </si>
-  <si>
-    <t>definitely send this one before subscribing to anything</t>
   </si>
 </sst>
 </file>
@@ -921,10 +915,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AA65"/>
+  <dimension ref="A1:AA64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F9" workbookViewId="0">
-      <selection activeCell="M35" sqref="M35"/>
+    <sheetView tabSelected="1" topLeftCell="F21" workbookViewId="0">
+      <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1506,41 +1500,38 @@
       <c r="D34" t="s">
         <v>32</v>
       </c>
-      <c r="I34">
-        <v>3</v>
-      </c>
-      <c r="J34" t="s">
-        <v>81</v>
-      </c>
-      <c r="K34" t="s">
-        <v>163</v>
-      </c>
-      <c r="L34" t="s">
-        <v>148</v>
-      </c>
-      <c r="M34" t="s">
-        <v>164</v>
-      </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C35" s="1"/>
       <c r="D35" t="s">
         <v>33</v>
       </c>
+      <c r="I35">
+        <v>16</v>
+      </c>
+      <c r="J35" t="s">
+        <v>88</v>
+      </c>
+      <c r="K35" t="s">
+        <v>111</v>
+      </c>
+      <c r="L35" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C36" s="1"/>
       <c r="I36">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J36" t="s">
-        <v>88</v>
+        <v>45</v>
       </c>
       <c r="K36" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="L36" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.3">
@@ -1557,98 +1548,98 @@
         <v>24</v>
       </c>
       <c r="I37">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J37" t="s">
-        <v>45</v>
+        <v>89</v>
       </c>
       <c r="K37" t="s">
-        <v>109</v>
+        <v>150</v>
       </c>
       <c r="L37" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C38" s="1"/>
       <c r="I38">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J38" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="K38" t="s">
-        <v>150</v>
+        <v>110</v>
       </c>
       <c r="L38" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I39">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J39" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K39" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="L39" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I40">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J40" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K40" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="L40" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I41">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J41" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="K41" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L41" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I42">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J42" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K42" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="L42" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I43">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J43" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K43" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="L43" t="s">
         <v>148</v>
@@ -1656,13 +1647,13 @@
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I44">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J44" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K44" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="L44" t="s">
         <v>148</v>
@@ -1670,13 +1661,13 @@
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I45">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J45" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="K45" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="L45" t="s">
         <v>148</v>
@@ -1684,13 +1675,13 @@
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I46">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J46" t="s">
-        <v>97</v>
+        <v>140</v>
       </c>
       <c r="K46" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="L46" t="s">
         <v>148</v>
@@ -1698,13 +1689,13 @@
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I47">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J47" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="K47" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="L47" t="s">
         <v>148</v>
@@ -1712,13 +1703,13 @@
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I48">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J48" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="K48" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="L48" t="s">
         <v>148</v>
@@ -1726,13 +1717,13 @@
     </row>
     <row r="49" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I49">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J49" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="K49" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="L49" t="s">
         <v>148</v>
@@ -1740,41 +1731,41 @@
     </row>
     <row r="50" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I50">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J50" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="K50" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="L50" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="51" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I51">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J51" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="K51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="L51" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="52" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I52">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J52" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K52" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="L52" t="s">
         <v>148</v>
@@ -1782,13 +1773,13 @@
     </row>
     <row r="53" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I53">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J53" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="K53" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L53" t="s">
         <v>148</v>
@@ -1796,13 +1787,13 @@
     </row>
     <row r="54" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I54">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J54" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K54" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="L54" t="s">
         <v>148</v>
@@ -1810,13 +1801,13 @@
     </row>
     <row r="55" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I55">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J55" t="s">
-        <v>132</v>
-      </c>
-      <c r="K55" t="s">
-        <v>127</v>
+        <v>133</v>
+      </c>
+      <c r="K55" s="10" t="s">
+        <v>128</v>
       </c>
       <c r="L55" t="s">
         <v>148</v>
@@ -1824,27 +1815,27 @@
     </row>
     <row r="56" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I56">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J56" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="K56" s="10" t="s">
-        <v>128</v>
+        <v>152</v>
       </c>
       <c r="L56" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="57" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I57">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J57" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="K57" s="10" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="L57" t="s">
         <v>149</v>
@@ -1852,13 +1843,13 @@
     </row>
     <row r="58" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I58">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J58" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="K58" s="10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="L58" t="s">
         <v>149</v>
@@ -1866,13 +1857,13 @@
     </row>
     <row r="59" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I59">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J59" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="K59" s="10" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="L59" t="s">
         <v>149</v>
@@ -1880,27 +1871,27 @@
     </row>
     <row r="60" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I60">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J60" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="K60" s="10" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="L60" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="61" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I61">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J61" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="K61" s="10" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L61" t="s">
         <v>148</v>
@@ -1908,13 +1899,13 @@
     </row>
     <row r="62" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I62">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J62" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="K62" s="10" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="L62" t="s">
         <v>148</v>
@@ -1922,13 +1913,13 @@
     </row>
     <row r="63" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I63">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J63" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="K63" s="10" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="L63" t="s">
         <v>148</v>
@@ -1936,29 +1927,15 @@
     </row>
     <row r="64" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I64">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J64" t="s">
-        <v>147</v>
-      </c>
-      <c r="K64" s="10" t="s">
-        <v>159</v>
+        <v>160</v>
+      </c>
+      <c r="K64" t="s">
+        <v>161</v>
       </c>
       <c r="L64" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="65" spans="9:12" x14ac:dyDescent="0.3">
-      <c r="I65">
-        <v>45</v>
-      </c>
-      <c r="J65" t="s">
-        <v>160</v>
-      </c>
-      <c r="K65" t="s">
-        <v>161</v>
-      </c>
-      <c r="L65" t="s">
         <v>148</v>
       </c>
     </row>

</xml_diff>